<commit_message>
Adding naive, ml, and neural net models as well as data prep code.
</commit_message>
<xml_diff>
--- a/Michelin_List.xlsx
+++ b/Michelin_List.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evanmoh/Desktop/540_deeplearning/Final Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9454D834-B41A-6F45-A736-7E3CD4154D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071CD139-1846-FF4E-B66B-91F88FAAF04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="-11480" windowWidth="38400" windowHeight="19940" xr2:uid="{FA37D46F-08E8-3440-B659-51299C00E0CC}"/>
+    <workbookView xWindow="6400" yWindow="2460" windowWidth="30240" windowHeight="17720" xr2:uid="{FA37D46F-08E8-3440-B659-51299C00E0CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$180</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$268</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1415" uniqueCount="377">
   <si>
     <t>Restaurant Name</t>
   </si>
@@ -1110,13 +1110,73 @@
   </si>
   <si>
     <t>Seafood/Italian</t>
+  </si>
+  <si>
+    <t>Localis</t>
+  </si>
+  <si>
+    <t>Holbox</t>
+  </si>
+  <si>
+    <t>Los Angels</t>
+  </si>
+  <si>
+    <t>Noksu</t>
+  </si>
+  <si>
+    <t>Sushi Noz</t>
+  </si>
+  <si>
+    <t>Kin Khao</t>
+  </si>
+  <si>
+    <t>Thai</t>
+  </si>
+  <si>
+    <t>Niku Steakhouse</t>
+  </si>
+  <si>
+    <t>Le Coucou</t>
+  </si>
+  <si>
+    <t>Victoria &amp; Albert's</t>
+  </si>
+  <si>
+    <t>Somni</t>
+  </si>
+  <si>
+    <t>Sorekara</t>
+  </si>
+  <si>
+    <t>Sons &amp; Daughters</t>
+  </si>
+  <si>
+    <t>Kiln</t>
+  </si>
+  <si>
+    <t>Vespertine</t>
+  </si>
+  <si>
+    <t>Nari</t>
+  </si>
+  <si>
+    <t>Ssal</t>
+  </si>
+  <si>
+    <t>Corima</t>
+  </si>
+  <si>
+    <t>Bom</t>
+  </si>
+  <si>
+    <t>Culver City</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1137,6 +1197,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1498,10 +1564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BFD391E-E0C2-F746-8AB9-36559EE4F7FD}">
-  <dimension ref="A1:N266"/>
+  <dimension ref="A1:N283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F203" sqref="F203"/>
+    <sheetView tabSelected="1" topLeftCell="A273" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E281" sqref="E281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6856,8 +6922,349 @@
         <v>21</v>
       </c>
     </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A267" t="s">
+        <v>357</v>
+      </c>
+      <c r="B267">
+        <v>1</v>
+      </c>
+      <c r="C267" t="s">
+        <v>339</v>
+      </c>
+      <c r="D267" t="s">
+        <v>236</v>
+      </c>
+      <c r="E267" t="s">
+        <v>19</v>
+      </c>
+      <c r="F267" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A268" t="s">
+        <v>358</v>
+      </c>
+      <c r="B268">
+        <v>1</v>
+      </c>
+      <c r="C268" t="s">
+        <v>359</v>
+      </c>
+      <c r="D268" t="s">
+        <v>236</v>
+      </c>
+      <c r="E268" t="s">
+        <v>41</v>
+      </c>
+      <c r="F268" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A269" t="s">
+        <v>360</v>
+      </c>
+      <c r="B269">
+        <v>1</v>
+      </c>
+      <c r="C269" t="s">
+        <v>92</v>
+      </c>
+      <c r="D269" t="s">
+        <v>93</v>
+      </c>
+      <c r="E269" t="s">
+        <v>99</v>
+      </c>
+      <c r="F269" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A270" t="s">
+        <v>361</v>
+      </c>
+      <c r="B270">
+        <v>2</v>
+      </c>
+      <c r="C270" t="s">
+        <v>92</v>
+      </c>
+      <c r="D270" t="s">
+        <v>93</v>
+      </c>
+      <c r="E270" t="s">
+        <v>18</v>
+      </c>
+      <c r="F270" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A271" t="s">
+        <v>362</v>
+      </c>
+      <c r="B271">
+        <v>1</v>
+      </c>
+      <c r="C271" t="s">
+        <v>270</v>
+      </c>
+      <c r="D271" t="s">
+        <v>236</v>
+      </c>
+      <c r="E271" t="s">
+        <v>363</v>
+      </c>
+      <c r="F271" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A272" t="s">
+        <v>364</v>
+      </c>
+      <c r="B272">
+        <v>1</v>
+      </c>
+      <c r="C272" t="s">
+        <v>270</v>
+      </c>
+      <c r="D272" t="s">
+        <v>236</v>
+      </c>
+      <c r="E272" t="s">
+        <v>17</v>
+      </c>
+      <c r="F272" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A273" t="s">
+        <v>365</v>
+      </c>
+      <c r="B273">
+        <v>1</v>
+      </c>
+      <c r="C273" t="s">
+        <v>92</v>
+      </c>
+      <c r="D273" t="s">
+        <v>93</v>
+      </c>
+      <c r="E273" t="s">
+        <v>35</v>
+      </c>
+      <c r="F273" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A274" t="s">
+        <v>366</v>
+      </c>
+      <c r="B274">
+        <v>1</v>
+      </c>
+      <c r="C274" t="s">
+        <v>170</v>
+      </c>
+      <c r="D274" t="s">
+        <v>167</v>
+      </c>
+      <c r="E274" t="s">
+        <v>19</v>
+      </c>
+      <c r="F274" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A275" t="s">
+        <v>367</v>
+      </c>
+      <c r="B275">
+        <v>3</v>
+      </c>
+      <c r="C275" t="s">
+        <v>292</v>
+      </c>
+      <c r="D275" t="s">
+        <v>236</v>
+      </c>
+      <c r="E275" t="s">
+        <v>19</v>
+      </c>
+      <c r="F275" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A276" t="s">
+        <v>368</v>
+      </c>
+      <c r="B276">
+        <v>2</v>
+      </c>
+      <c r="C276" t="s">
+        <v>170</v>
+      </c>
+      <c r="D276" t="s">
+        <v>167</v>
+      </c>
+      <c r="E276" t="s">
+        <v>18</v>
+      </c>
+      <c r="F276" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A277" t="s">
+        <v>369</v>
+      </c>
+      <c r="B277">
+        <v>2</v>
+      </c>
+      <c r="C277" t="s">
+        <v>270</v>
+      </c>
+      <c r="D277" t="s">
+        <v>236</v>
+      </c>
+      <c r="E277" t="s">
+        <v>19</v>
+      </c>
+      <c r="F277" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A278" t="s">
+        <v>370</v>
+      </c>
+      <c r="B278">
+        <v>2</v>
+      </c>
+      <c r="C278" t="s">
+        <v>270</v>
+      </c>
+      <c r="D278" t="s">
+        <v>236</v>
+      </c>
+      <c r="E278" t="s">
+        <v>19</v>
+      </c>
+      <c r="F278" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A279" t="s">
+        <v>371</v>
+      </c>
+      <c r="B279">
+        <v>2</v>
+      </c>
+      <c r="C279" t="s">
+        <v>376</v>
+      </c>
+      <c r="D279" t="s">
+        <v>236</v>
+      </c>
+      <c r="E279" t="s">
+        <v>19</v>
+      </c>
+      <c r="F279" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A280" t="s">
+        <v>372</v>
+      </c>
+      <c r="B280">
+        <v>1</v>
+      </c>
+      <c r="C280" t="s">
+        <v>270</v>
+      </c>
+      <c r="D280" t="s">
+        <v>236</v>
+      </c>
+      <c r="E280" t="s">
+        <v>363</v>
+      </c>
+      <c r="F280" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A281" t="s">
+        <v>373</v>
+      </c>
+      <c r="B281">
+        <v>1</v>
+      </c>
+      <c r="C281" t="s">
+        <v>270</v>
+      </c>
+      <c r="D281" t="s">
+        <v>236</v>
+      </c>
+      <c r="E281" t="s">
+        <v>99</v>
+      </c>
+      <c r="F281" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A282" t="s">
+        <v>374</v>
+      </c>
+      <c r="B282">
+        <v>1</v>
+      </c>
+      <c r="C282" t="s">
+        <v>92</v>
+      </c>
+      <c r="D282" t="s">
+        <v>93</v>
+      </c>
+      <c r="E282" t="s">
+        <v>41</v>
+      </c>
+      <c r="F282" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A283" t="s">
+        <v>375</v>
+      </c>
+      <c r="B283">
+        <v>1</v>
+      </c>
+      <c r="C283" t="s">
+        <v>92</v>
+      </c>
+      <c r="D283" t="s">
+        <v>93</v>
+      </c>
+      <c r="E283" t="s">
+        <v>99</v>
+      </c>
+      <c r="F283" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F180" xr:uid="{1BFD391E-E0C2-F746-8AB9-36559EE4F7FD}"/>
+  <autoFilter ref="A1:F268" xr:uid="{1BFD391E-E0C2-F746-8AB9-36559EE4F7FD}"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>